<commit_message>
Modification diagramme de classe
</commit_message>
<xml_diff>
--- a/documents/analyse_uml/usecase_textuel/use_case_sonder/Creersondage.xlsx
+++ b/documents/analyse_uml/usecase_textuel/use_case_sonder/Creersondage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Quideance\documents\analyse_uml\usecase_textuel\use_case_questionner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Quideance\documents\analyse_uml\usecase_textuel\use_case_sonder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5368A347-F218-4E7B-8E47-53B21776B178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26025233-B946-472C-9CAB-E3EB582D61B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27600" windowHeight="15630" xr2:uid="{A6AFA233-EB2B-47F1-B1C2-7A20F721B039}"/>
   </bookViews>
@@ -167,6 +167,43 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>E3) Erreur enregistrement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+a lieu au point 6) du nominal
+Quideance affiche un message d'erreur adéquat
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>On sort du USE CASE sur un échec</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>NOM DU USE CASE</t>
     </r>
     <r>
@@ -177,7 +214,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> : créerquestionner</t>
+      <t xml:space="preserve"> : créersondage</t>
     </r>
   </si>
   <si>
@@ -222,7 +259,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> : créer un formulaire (question, réponse)</t>
+      <t xml:space="preserve"> : créer un sondage (question, réponse)</t>
     </r>
   </si>
   <si>
@@ -251,51 +288,14 @@
 - la fonctionnalité "Se déconnecter" est accessible
 - la fonctionnalité "Administration" est accessible
 - la fonctionnalité "Accueil" est accessible
-- la fonctionnalité "Ajouter un questionnaire" est accessible</t>
-    </r>
-  </si>
-  <si>
-    <t>1) L'administrateur clique sur le bouton "Ajouter un questionnaire"</t>
-  </si>
-  <si>
-    <t>2) Quideance redirige vers la page de création d'un nouveau questionnaire</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E3) Erreur enregistrement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-a lieu au point 6) du nominal
-Quideance affiche un message d'erreur adéquat
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>On sort du USE CASE sur un échec</t>
-    </r>
+- la fonctionnalité "Ajouter un sondage" est accessible</t>
+    </r>
+  </si>
+  <si>
+    <t>1) L'administrateur clique sur le bouton "Ajouter un sondage"</t>
+  </si>
+  <si>
+    <t>2) Quideance redirige vers la page de création d'un nouveau sondage</t>
   </si>
 </sst>
 </file>
@@ -421,10 +421,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -438,6 +434,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1D72FA5-1A7B-44E8-9361-94AB399D546A}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D9:D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,32 +768,32 @@
   <sheetData>
     <row r="1" spans="1:4" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" ht="120.75" x14ac:dyDescent="0.25">
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" ht="105.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="3"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -804,7 +804,7 @@
     </row>
     <row r="5" spans="1:4" ht="90.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
@@ -813,10 +813,10 @@
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="7"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -840,18 +840,18 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>